<commit_message>
Optimizes 2 params for Pearson correlation (#17)
* nelderMead runs

* nelderMead runs with 2 vars

* Optimized Pearson

* Optimizes 2 params for Pearson correlation

Co-authored-by: Gilles Fabre <gillesfabre34@gmail.com>
</commit_message>
<xml_diff>
--- a/src/core/mocks/code-snippets/dataset.xlsx
+++ b/src/core/mocks/code-snippets/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/Documents/projets/genese/metrics/src/core/mocks/code-snippets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B1F290-BB08-F34B-A70C-3035242A529A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B0E8E7-0037-F742-B358-9E7DACB3E262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41480" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{6B2507F4-2ED4-784C-80A2-5B5CA1CAB9E0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{6B2507F4-2ED4-784C-80A2-5B5CA1CAB9E0}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>measure</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>three</t>
+  </si>
+  <si>
+    <t>two</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E401E57-2C53-E249-A7ED-8E36F62BE131}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,15 +478,23 @@
         <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>9</v>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Still runs when no trace()
</commit_message>
<xml_diff>
--- a/src/core/mocks/code-snippets/dataset.xlsx
+++ b/src/core/mocks/code-snippets/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/Documents/projets/genese/metrics/src/core/mocks/code-snippets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69CE570-7252-1244-A7AE-AF87E747C54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020A717B-87CF-264D-90BE-83BF36538231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{6B2507F4-2ED4-784C-80A2-5B5CA1CAB9E0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{6B2507F4-2ED4-784C-80A2-5B5CA1CAB9E0}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>measure</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>two</t>
-  </si>
-  <si>
-    <t>four</t>
   </si>
 </sst>
 </file>
@@ -450,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E401E57-2C53-E249-A7ED-8E36F62BE131}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,14 +497,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
v0.1.0 Added dynamic lines (#25)
* Refacto get score

* Refacto global algo

* Still bugging

* No-optimization

* Unstable

* Still runs when no trace()

* Adding startTracing()

* Fixed bug with export {}

* Added startTrace()

* startTracing() runs

* Tracing runs

* Flags only outside traceProcess()

* Wrong results for genese-cpx

* All runs

* Cleaned code

* v0.1.0 Added dynamic lines

Co-authored-by: Gilles Fabre <gillesfabre34@gmail.com>
</commit_message>
<xml_diff>
--- a/src/core/mocks/code-snippets/dataset.xlsx
+++ b/src/core/mocks/code-snippets/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utilisateur/Documents/projets/genese/metrics/src/core/mocks/code-snippets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B0E8E7-0037-F742-B358-9E7DACB3E262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020A717B-87CF-264D-90BE-83BF36538231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{6B2507F4-2ED4-784C-80A2-5B5CA1CAB9E0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{6B2507F4-2ED4-784C-80A2-5B5CA1CAB9E0}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>